<commit_message>
finished the result excel file
</commit_message>
<xml_diff>
--- a/project_recommender2021/results_project.xlsx
+++ b/project_recommender2021/results_project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\iCloudDrive\UNI\SoSE_21\Recommender Systems\Project\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\recommender2021\project_recommender2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0134D9-B158-4579-A43F-813821A98E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6019DAE4-5FF8-4119-B4A0-1545C92BB1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{08C42D0C-B7A5-41F5-AA4C-F743BA837BF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{08C42D0C-B7A5-41F5-AA4C-F743BA837BF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="475">
   <si>
     <t>Tags</t>
   </si>
@@ -1165,6 +1165,310 @@
   </si>
   <si>
     <t>All Algorithms / Same Weight</t>
+  </si>
+  <si>
+    <t>Drugstore Cowboy</t>
+  </si>
+  <si>
+    <t>Killing Zoe</t>
+  </si>
+  <si>
+    <t>Training Day</t>
+  </si>
+  <si>
+    <t>Taxi Driver</t>
+  </si>
+  <si>
+    <t>GoodFellas</t>
+  </si>
+  <si>
+    <t>Raging Bull</t>
+  </si>
+  <si>
+    <t>Code of Silence</t>
+  </si>
+  <si>
+    <t>Below</t>
+  </si>
+  <si>
+    <t>Mr. Sardonicus</t>
+  </si>
+  <si>
+    <t>Wings of Courage</t>
+  </si>
+  <si>
+    <t>Trick</t>
+  </si>
+  <si>
+    <t>Ralphie May: Imperfectly Yours</t>
+  </si>
+  <si>
+    <t>Wild Card</t>
+  </si>
+  <si>
+    <t>Finding Amanda</t>
+  </si>
+  <si>
+    <t>Perry Mason: The Case of the Defiant Daughter</t>
+  </si>
+  <si>
+    <t>Dolan's Cadillac</t>
+  </si>
+  <si>
+    <t>The Departed</t>
+  </si>
+  <si>
+    <t>The Wolf of Wall Street</t>
+  </si>
+  <si>
+    <t>Twinkle</t>
+  </si>
+  <si>
+    <t>Last Orders</t>
+  </si>
+  <si>
+    <t>A Taste of Honey</t>
+  </si>
+  <si>
+    <t>American Pastoral</t>
+  </si>
+  <si>
+    <t>Witness for the Prosecution</t>
+  </si>
+  <si>
+    <t>The Scarlet Letter</t>
+  </si>
+  <si>
+    <t>5 Card Stud</t>
+  </si>
+  <si>
+    <t>My Boyfriend's Back</t>
+  </si>
+  <si>
+    <t>Arlington Road</t>
+  </si>
+  <si>
+    <t>An American Haunting</t>
+  </si>
+  <si>
+    <t>The Lost Thing</t>
+  </si>
+  <si>
+    <t>Carver</t>
+  </si>
+  <si>
+    <t>Crane World</t>
+  </si>
+  <si>
+    <t>The Marshal of Finland</t>
+  </si>
+  <si>
+    <t>The Princess Bride</t>
+  </si>
+  <si>
+    <t>Romancing the Stone</t>
+  </si>
+  <si>
+    <t>Boys and Girls</t>
+  </si>
+  <si>
+    <t>Allied</t>
+  </si>
+  <si>
+    <t>The Evening Star</t>
+  </si>
+  <si>
+    <t>Chocolat</t>
+  </si>
+  <si>
+    <t>City Lights</t>
+  </si>
+  <si>
+    <t>Beautiful Girls</t>
+  </si>
+  <si>
+    <t>Return to Me</t>
+  </si>
+  <si>
+    <t>Sleepless in Seattle</t>
+  </si>
+  <si>
+    <t>Benny &amp; Joon</t>
+  </si>
+  <si>
+    <t>The Games Maker</t>
+  </si>
+  <si>
+    <t>Miss Peregrine's Home for Peculiar Children</t>
+  </si>
+  <si>
+    <t>Sesame Street Presents Follow That Bird</t>
+  </si>
+  <si>
+    <t>The Water Horse</t>
+  </si>
+  <si>
+    <t>The Butterfly Ball</t>
+  </si>
+  <si>
+    <t>Step Up All In</t>
+  </si>
+  <si>
+    <t>The Amati Girls</t>
+  </si>
+  <si>
+    <t>Cool Runnings</t>
+  </si>
+  <si>
+    <t>Children Underground</t>
+  </si>
+  <si>
+    <t>Nine Months</t>
+  </si>
+  <si>
+    <t>The NeverEnding Story</t>
+  </si>
+  <si>
+    <t>Table No. 21</t>
+  </si>
+  <si>
+    <t>Quiz</t>
+  </si>
+  <si>
+    <t>Liar Game: Reborn</t>
+  </si>
+  <si>
+    <t>Quintet</t>
+  </si>
+  <si>
+    <t>Brainscan</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings: 
+The Fellowship of the Ring</t>
+  </si>
+  <si>
+    <t>E.T. the Extra-Terrestrial</t>
+  </si>
+  <si>
+    <t>Jumanji</t>
+  </si>
+  <si>
+    <t>The Rocketeer</t>
+  </si>
+  <si>
+    <t>Honey, I Shrunk the Kids</t>
+  </si>
+  <si>
+    <t>The Pagemaster</t>
+  </si>
+  <si>
+    <t>Beauty and the Beast</t>
+  </si>
+  <si>
+    <t>Harry Potter and the Philosopher's Stone</t>
+  </si>
+  <si>
+    <t>The Wizard of Oz</t>
+  </si>
+  <si>
+    <t>Hangover</t>
+  </si>
+  <si>
+    <t>Last Vegas</t>
+  </si>
+  <si>
+    <t>Very Bad Things</t>
+  </si>
+  <si>
+    <t>Hal</t>
+  </si>
+  <si>
+    <t>Finding Nemo</t>
+  </si>
+  <si>
+    <t>Dog Eat Dog</t>
+  </si>
+  <si>
+    <t>Guarding Tess</t>
+  </si>
+  <si>
+    <t>For Love or Money</t>
+  </si>
+  <si>
+    <t>Multiplicity</t>
+  </si>
+  <si>
+    <t>Floating</t>
+  </si>
+  <si>
+    <t>The Wedding Ringer</t>
+  </si>
+  <si>
+    <t>The Hangover Part II</t>
+  </si>
+  <si>
+    <t>The Hangover Part III</t>
+  </si>
+  <si>
+    <t>Starsky &amp; Hutch</t>
+  </si>
+  <si>
+    <t>War Dogs</t>
+  </si>
+  <si>
+    <t>Superbad</t>
+  </si>
+  <si>
+    <t>American Pie</t>
+  </si>
+  <si>
+    <t>Dope</t>
+  </si>
+  <si>
+    <t>Me and Earl and the Dying Girl</t>
+  </si>
+  <si>
+    <t>The Spectacular Now</t>
+  </si>
+  <si>
+    <t>A Walk to Remember</t>
+  </si>
+  <si>
+    <t>The 40 Year Old Virgin</t>
+  </si>
+  <si>
+    <t>This Is the End</t>
+  </si>
+  <si>
+    <t>Hooking Up</t>
+  </si>
+  <si>
+    <t>House Party: Tonight's the Night</t>
+  </si>
+  <si>
+    <t>American Graffiti</t>
+  </si>
+  <si>
+    <t>Club Sandwich</t>
+  </si>
+  <si>
+    <t>Do I Have to Take Care of Everything?</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Adventureland</t>
+  </si>
+  <si>
+    <t>Clear History</t>
+  </si>
+  <si>
+    <t>Keeping Up with the Joneses</t>
+  </si>
+  <si>
+    <t>Too few ratings</t>
   </si>
 </sst>
 </file>
@@ -1262,7 +1566,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1303,9 +1607,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1339,6 +1640,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1657,10 +1967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF637B4-0E5C-43C4-929E-28FE0E130176}">
-  <dimension ref="A1:J141"/>
+  <dimension ref="A1:J191"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="D166" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,165 +1989,173 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="29" t="s">
         <v>324</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
-        <f>AVERAGE(B14,B23,B32,B41,B50,B59,B68,B77,B86,B95,B104,B113,B122,B131)</f>
-        <v>3.2857142857142856</v>
-      </c>
-      <c r="C2" s="1">
-        <f t="shared" ref="C2:J2" si="0">AVERAGE(C14,C23,C32,C41,C50,C59,C68,C77,C86,C95,C104,C113)</f>
-        <v>1.8333333333333333</v>
-      </c>
-      <c r="D2" s="1">
-        <f>AVERAGE(D14,D23,D32,D41,D50,D59,D68,D77,D86,D95,D104,D113)</f>
-        <v>0.7</v>
-      </c>
-      <c r="E2" s="1">
+        <f>AVERAGE(B14,B23,B32,B41,B50,B59,B68,B77,B86,B95,B104,B113,B122,B131,B140,B150,B160,B170,B181,B190)</f>
+        <v>3.3</v>
+      </c>
+      <c r="C2" s="2">
+        <f t="shared" ref="C2:J2" si="0">AVERAGE(C14,C23,C32,C41,C50,C59,C68,C77,C86,C95,C104,C113,C122,C131,C140,C150,C160,C170,C181,C190)</f>
+        <v>1.3157894736842106</v>
+      </c>
+      <c r="D2" s="2">
         <f t="shared" si="0"/>
-        <v>2.8333333333333335</v>
-      </c>
-      <c r="F2" s="1">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="E2" s="2">
         <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="G2" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F2" s="2">
         <f t="shared" si="0"/>
-        <v>3.5</v>
-      </c>
-      <c r="H2" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="G2" s="2">
         <f t="shared" si="0"/>
-        <v>3.9090909090909092</v>
-      </c>
-      <c r="I2" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="H2" s="2">
         <f t="shared" si="0"/>
-        <v>3.5</v>
-      </c>
-      <c r="J2" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="I2" s="2">
         <f t="shared" si="0"/>
-        <v>3.6363636363636362</v>
+        <v>3.5333333333333332</v>
+      </c>
+      <c r="J2" s="2">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="29" t="s">
         <v>325</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
-        <f>AVERAGE(B15,B24,B33,B42,B51,B60,B69,B78,B87,B96,B105,B114,B123,B132)/2</f>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="C4" s="1">
-        <f>AVERAGE(C15,C24,C33,C42,C51,C60,C69,C78,C87,C96,C105,C114)/2</f>
-        <v>0.45454545454545453</v>
-      </c>
-      <c r="D4" s="1">
-        <f>AVERAGE(D15,D24,D33,D42,D51,D60,D69,D78,D87,D96,D105,D114)/2</f>
-        <v>0.45</v>
-      </c>
-      <c r="E4" s="1">
-        <f>AVERAGE(E15,E24,E33,E42,E51,E60,E69,E78,E87,E96,E105,E114)/2</f>
+        <f>AVERAGE(B15,B24,B33,B42,B51,B60,B69,B78,B87,B96,B105,B114,B123,B132,B141,B151,B161,B171,B182,B191)/2</f>
+        <v>0.4</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:J4" si="1">AVERAGE(C15,C24,C33,C42,C51,C60,C69,C78,C87,C96,C105,C114,C123,C132,C141,C151,C161,C171,C182,C191)/2</f>
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.65789473684210531</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.60526315789473684</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F4" s="1">
-        <f>AVERAGE(F15,F24,F33,F42,F51,F60,F69,F78,F87,F96,F105,F114)/2</f>
-        <v>0.45454545454545453</v>
-      </c>
-      <c r="G4" s="1">
-        <f>AVERAGE(G15,G24,G33,G42,G51,G60,G69,G78,G87,G96,G105,G114)/2</f>
-        <v>0.31818181818181818</v>
-      </c>
-      <c r="H4" s="1">
-        <f>AVERAGE(H15,H24,H33,H42,H51,H60,H69,H78,H87,H96,H105,H114)/2</f>
-        <v>0.2</v>
-      </c>
-      <c r="I4" s="1">
-        <f>AVERAGE(I15,I24,I33,I42,I51,I60,I69,I78,I87,I96,I105,I114)/2</f>
-        <v>0.35</v>
-      </c>
-      <c r="J4" s="1">
-        <f>AVERAGE(J15,J24,J33,J42,J51,J60,J69,J78,J87,J96,J105,J114)/2</f>
-        <v>0.35</v>
+      <c r="I4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <f>B2+B4</f>
-        <v>3.5714285714285712</v>
+        <v>3.6999999999999997</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6:J6" si="1">C2+C4</f>
-        <v>2.2878787878787876</v>
+        <f t="shared" ref="C6:J6" si="2">C2+C4</f>
+        <v>1.6769005847953218</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="1"/>
-        <v>1.1499999999999999</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="1"/>
-        <v>3.166666666666667</v>
+        <f t="shared" si="2"/>
+        <v>2.6750000000000003</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="1"/>
-        <v>2.9545454545454546</v>
+        <f t="shared" si="2"/>
+        <v>2.7078947368421051</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="1"/>
-        <v>3.8181818181818183</v>
+        <f t="shared" si="2"/>
+        <v>3.8052631578947369</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="1"/>
-        <v>4.1090909090909093</v>
+        <f t="shared" si="2"/>
+        <v>4.083333333333333</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="1"/>
-        <v>3.85</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="1"/>
-        <v>3.9863636363636363</v>
+        <f t="shared" si="2"/>
+        <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="29" t="s">
         <v>4</v>
       </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="28">
+      <c r="A8" s="27">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1858,7 +2176,7 @@
       <c r="G8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>373</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -2093,12 +2411,20 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="29" t="s">
         <v>66</v>
       </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28">
+      <c r="A17" s="27">
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2119,7 +2445,7 @@
       <c r="G17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="17" t="s">
         <v>373</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -2354,9 +2680,17 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="29" t="s">
         <v>67</v>
       </c>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
     </row>
     <row r="26" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -2380,7 +2714,7 @@
       <c r="G26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H26" s="18" t="s">
+      <c r="H26" s="17" t="s">
         <v>373</v>
       </c>
       <c r="I26" s="1" t="s">
@@ -2615,9 +2949,17 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="29" t="s">
         <v>87</v>
       </c>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
     </row>
     <row r="35" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
@@ -2641,7 +2983,7 @@
       <c r="G35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H35" s="18" t="s">
+      <c r="H35" s="17" t="s">
         <v>373</v>
       </c>
       <c r="I35" s="1" t="s">
@@ -2876,9 +3218,17 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="29" t="s">
         <v>115</v>
       </c>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
     </row>
     <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
@@ -2902,7 +3252,7 @@
       <c r="G44" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H44" s="17" t="s">
         <v>373</v>
       </c>
       <c r="I44" s="1" t="s">
@@ -3137,9 +3487,17 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="29" t="s">
         <v>140</v>
       </c>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
     </row>
     <row r="53" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
@@ -3163,7 +3521,7 @@
       <c r="G53" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H53" s="18" t="s">
+      <c r="H53" s="17" t="s">
         <v>373</v>
       </c>
       <c r="I53" s="1" t="s">
@@ -3398,9 +3756,17 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="29" t="s">
         <v>203</v>
       </c>
+      <c r="C61" s="29"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="29"/>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
@@ -3424,7 +3790,7 @@
       <c r="G62" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H62" s="18" t="s">
+      <c r="H62" s="17" t="s">
         <v>373</v>
       </c>
       <c r="I62" s="1" t="s">
@@ -3434,7 +3800,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>5</v>
       </c>
@@ -3444,7 +3810,7 @@
       <c r="C63" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D63" s="19" t="s">
+      <c r="D63" s="30" t="s">
         <v>169</v>
       </c>
       <c r="E63" s="6" t="s">
@@ -3456,13 +3822,13 @@
       <c r="G63" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H63" s="19" t="s">
+      <c r="H63" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="I63" s="19" t="s">
+      <c r="I63" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="J63" s="19" t="s">
+      <c r="J63" s="30" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3476,7 +3842,7 @@
       <c r="C64" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D64" s="18"/>
+      <c r="D64" s="30"/>
       <c r="E64" s="6" t="s">
         <v>171</v>
       </c>
@@ -3486,9 +3852,9 @@
       <c r="G64" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="H64" s="18"/>
-      <c r="I64" s="18"/>
-      <c r="J64" s="18"/>
+      <c r="H64" s="30"/>
+      <c r="I64" s="30"/>
+      <c r="J64" s="30"/>
     </row>
     <row r="65" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
@@ -3500,8 +3866,8 @@
       <c r="C65" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="D65" s="18"/>
-      <c r="E65" s="17">
+      <c r="D65" s="30"/>
+      <c r="E65" s="16">
         <v>911</v>
       </c>
       <c r="F65" s="4" t="s">
@@ -3510,9 +3876,9 @@
       <c r="G65" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="H65" s="18"/>
-      <c r="I65" s="18"/>
-      <c r="J65" s="18"/>
+      <c r="H65" s="30"/>
+      <c r="I65" s="30"/>
+      <c r="J65" s="30"/>
     </row>
     <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
@@ -3524,7 +3890,7 @@
       <c r="C66" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D66" s="18"/>
+      <c r="D66" s="30"/>
       <c r="E66" s="15" t="s">
         <v>172</v>
       </c>
@@ -3534,9 +3900,9 @@
       <c r="G66" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="H66" s="18"/>
-      <c r="I66" s="18"/>
-      <c r="J66" s="18"/>
+      <c r="H66" s="30"/>
+      <c r="I66" s="30"/>
+      <c r="J66" s="30"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
@@ -3548,7 +3914,7 @@
       <c r="C67" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D67" s="18"/>
+      <c r="D67" s="30"/>
       <c r="E67" s="6" t="s">
         <v>166</v>
       </c>
@@ -3558,9 +3924,9 @@
       <c r="G67" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
-      <c r="J67" s="18"/>
+      <c r="H67" s="30"/>
+      <c r="I67" s="30"/>
+      <c r="J67" s="30"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -3603,9 +3969,17 @@
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="29" t="s">
         <v>182</v>
       </c>
+      <c r="C70" s="29"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="29"/>
+      <c r="F70" s="29"/>
+      <c r="G70" s="29"/>
+      <c r="H70" s="29"/>
+      <c r="I70" s="29"/>
+      <c r="J70" s="29"/>
     </row>
     <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
@@ -3629,7 +4003,7 @@
       <c r="G71" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H71" s="18" t="s">
+      <c r="H71" s="17" t="s">
         <v>373</v>
       </c>
       <c r="I71" s="1" t="s">
@@ -3861,9 +4235,17 @@
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="29" t="s">
         <v>209</v>
       </c>
+      <c r="C79" s="29"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29"/>
+      <c r="G79" s="29"/>
+      <c r="H79" s="29"/>
+      <c r="I79" s="29"/>
+      <c r="J79" s="29"/>
     </row>
     <row r="80" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
@@ -3887,7 +4269,7 @@
       <c r="G80" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H80" s="18" t="s">
+      <c r="H80" s="17" t="s">
         <v>373</v>
       </c>
       <c r="I80" s="1" t="s">
@@ -4098,48 +4480,48 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="18"/>
-      <c r="B88" s="18" t="s">
+      <c r="A88" s="17"/>
+      <c r="B88" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="C88" s="18"/>
-      <c r="D88" s="18"/>
-      <c r="E88" s="18"/>
-      <c r="F88" s="18"/>
-      <c r="G88" s="18"/>
-      <c r="H88" s="18"/>
-      <c r="I88" s="18"/>
-      <c r="J88" s="18"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="28"/>
+      <c r="F88" s="28"/>
+      <c r="G88" s="28"/>
+      <c r="H88" s="28"/>
+      <c r="I88" s="28"/>
+      <c r="J88" s="28"/>
     </row>
     <row r="89" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="18">
+      <c r="A89" s="17">
         <v>10</v>
       </c>
-      <c r="B89" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C89" s="18" t="s">
+      <c r="B89" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C89" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D89" s="18" t="s">
+      <c r="D89" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E89" s="18" t="s">
+      <c r="E89" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F89" s="18" t="s">
+      <c r="F89" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G89" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H89" s="18" t="s">
+      <c r="G89" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H89" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="I89" s="18" t="s">
+      <c r="I89" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="J89" s="19" t="s">
+      <c r="J89" s="18" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4147,31 +4529,31 @@
       <c r="A90" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B90" s="23" t="s">
+      <c r="B90" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="C90" s="23" t="s">
+      <c r="C90" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="D90" s="23" t="s">
+      <c r="D90" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="E90" s="23" t="s">
+      <c r="E90" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="F90" s="23" t="s">
+      <c r="F90" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="G90" s="23" t="s">
+      <c r="G90" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="H90" s="23" t="s">
+      <c r="H90" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="I90" s="23" t="s">
+      <c r="I90" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="J90" s="23" t="s">
+      <c r="J90" s="22" t="s">
         <v>232</v>
       </c>
     </row>
@@ -4179,31 +4561,31 @@
       <c r="A91" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B91" s="23" t="s">
+      <c r="B91" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="C91" s="20" t="s">
+      <c r="C91" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="D91" s="24" t="s">
+      <c r="D91" s="23" t="s">
         <v>240</v>
       </c>
-      <c r="E91" s="25" t="s">
+      <c r="E91" s="24" t="s">
         <v>245</v>
       </c>
-      <c r="F91" s="23" t="s">
+      <c r="F91" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="G91" s="23" t="s">
+      <c r="G91" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="H91" s="23" t="s">
+      <c r="H91" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="I91" s="23" t="s">
+      <c r="I91" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="J91" s="23" t="s">
+      <c r="J91" s="22" t="s">
         <v>236</v>
       </c>
     </row>
@@ -4211,31 +4593,31 @@
       <c r="A92" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B92" s="23" t="s">
+      <c r="B92" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="C92" s="23" t="s">
+      <c r="C92" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="D92" s="24" t="s">
+      <c r="D92" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="E92" s="24" t="s">
+      <c r="E92" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="F92" s="23" t="s">
+      <c r="F92" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="G92" s="23" t="s">
+      <c r="G92" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="H92" s="23" t="s">
+      <c r="H92" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="I92" s="23" t="s">
+      <c r="I92" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="J92" s="23" t="s">
+      <c r="J92" s="22" t="s">
         <v>250</v>
       </c>
     </row>
@@ -4243,31 +4625,31 @@
       <c r="A93" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B93" s="23" t="s">
+      <c r="B93" s="22" t="s">
         <v>235</v>
       </c>
-      <c r="C93" s="23" t="s">
+      <c r="C93" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="D93" s="25" t="s">
+      <c r="D93" s="24" t="s">
         <v>242</v>
       </c>
-      <c r="E93" s="24" t="s">
+      <c r="E93" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="F93" s="23" t="s">
+      <c r="F93" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="G93" s="23" t="s">
+      <c r="G93" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="H93" s="23" t="s">
+      <c r="H93" s="22" t="s">
         <v>252</v>
       </c>
-      <c r="I93" s="23" t="s">
+      <c r="I93" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="J93" s="23" t="s">
+      <c r="J93" s="22" t="s">
         <v>233</v>
       </c>
     </row>
@@ -4275,31 +4657,31 @@
       <c r="A94" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B94" s="23" t="s">
+      <c r="B94" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="C94" s="20" t="s">
+      <c r="C94" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="D94" s="25" t="s">
+      <c r="D94" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="E94" s="25" t="s">
+      <c r="E94" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="F94" s="23" t="s">
+      <c r="F94" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="G94" s="23" t="s">
+      <c r="G94" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="H94" s="23" t="s">
+      <c r="H94" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="I94" s="23" t="s">
+      <c r="I94" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="J94" s="23" t="s">
+      <c r="J94" s="22" t="s">
         <v>252</v>
       </c>
     </row>
@@ -4307,31 +4689,31 @@
       <c r="A95" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B95" s="18">
+      <c r="B95" s="17">
         <v>5</v>
       </c>
-      <c r="C95" s="18">
+      <c r="C95" s="17">
         <v>5</v>
       </c>
-      <c r="D95" s="18">
-        <v>1</v>
-      </c>
-      <c r="E95" s="18">
-        <v>1</v>
-      </c>
-      <c r="F95" s="18">
+      <c r="D95" s="17">
+        <v>1</v>
+      </c>
+      <c r="E95" s="17">
+        <v>1</v>
+      </c>
+      <c r="F95" s="17">
         <v>5</v>
       </c>
-      <c r="G95" s="18">
+      <c r="G95" s="17">
         <v>5</v>
       </c>
-      <c r="H95" s="18">
+      <c r="H95" s="17">
         <v>5</v>
       </c>
-      <c r="I95" s="18">
+      <c r="I95" s="17">
         <v>5</v>
       </c>
-      <c r="J95" s="18">
+      <c r="J95" s="17">
         <v>5</v>
       </c>
     </row>
@@ -4342,65 +4724,73 @@
       <c r="B96" s="1">
         <v>0</v>
       </c>
-      <c r="C96" s="18">
-        <v>0</v>
-      </c>
-      <c r="D96" s="18">
-        <v>1</v>
-      </c>
-      <c r="E96" s="18">
-        <v>1</v>
-      </c>
-      <c r="F96" s="18">
-        <v>0</v>
-      </c>
-      <c r="G96" s="18">
-        <v>0</v>
-      </c>
-      <c r="H96" s="18">
-        <v>0</v>
-      </c>
-      <c r="I96" s="18">
-        <v>0</v>
-      </c>
-      <c r="J96" s="18">
+      <c r="C96" s="17">
+        <v>0</v>
+      </c>
+      <c r="D96" s="17">
+        <v>1</v>
+      </c>
+      <c r="E96" s="17">
+        <v>1</v>
+      </c>
+      <c r="F96" s="17">
+        <v>0</v>
+      </c>
+      <c r="G96" s="17">
+        <v>0</v>
+      </c>
+      <c r="H96" s="17">
+        <v>0</v>
+      </c>
+      <c r="I96" s="17">
+        <v>0</v>
+      </c>
+      <c r="J96" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B97" s="18" t="s">
+      <c r="B97" s="28" t="s">
         <v>261</v>
       </c>
+      <c r="C97" s="28"/>
+      <c r="D97" s="28"/>
+      <c r="E97" s="28"/>
+      <c r="F97" s="28"/>
+      <c r="G97" s="28"/>
+      <c r="H97" s="28"/>
+      <c r="I97" s="28"/>
+      <c r="J97" s="28"/>
     </row>
     <row r="98" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="18">
+      <c r="A98" s="17">
         <v>11</v>
       </c>
-      <c r="B98" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C98" s="18" t="s">
+      <c r="B98" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D98" s="18" t="s">
+      <c r="D98" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E98" s="18" t="s">
+      <c r="E98" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F98" s="18" t="s">
+      <c r="F98" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G98" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H98" s="18" t="s">
+      <c r="G98" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H98" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="I98" s="18" t="s">
+      <c r="I98" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="J98" s="19" t="s">
+      <c r="J98" s="18" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4408,31 +4798,31 @@
       <c r="A99" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B99" s="24" t="s">
+      <c r="B99" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="C99" s="25" t="s">
+      <c r="C99" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="D99" s="24" t="s">
+      <c r="D99" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="E99" s="25" t="s">
+      <c r="E99" s="24" t="s">
         <v>273</v>
       </c>
-      <c r="F99" s="24" t="s">
+      <c r="F99" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="G99" s="23" t="s">
+      <c r="G99" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="H99" s="23" t="s">
+      <c r="H99" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="I99" s="24" t="s">
+      <c r="I99" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="J99" s="24" t="s">
+      <c r="J99" s="23" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4440,31 +4830,31 @@
       <c r="A100" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B100" s="24" t="s">
+      <c r="B100" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="C100" s="24" t="s">
+      <c r="C100" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="D100" s="23" t="s">
+      <c r="D100" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="E100" s="25" t="s">
+      <c r="E100" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="F100" s="23" t="s">
+      <c r="F100" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="G100" s="23" t="s">
+      <c r="G100" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="H100" s="23" t="s">
+      <c r="H100" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="I100" s="23" t="s">
+      <c r="I100" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="J100" s="23" t="s">
+      <c r="J100" s="22" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4472,31 +4862,31 @@
       <c r="A101" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B101" s="23" t="s">
+      <c r="B101" s="22" t="s">
         <v>264</v>
       </c>
-      <c r="C101" s="24" t="s">
+      <c r="C101" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D101" s="23" t="s">
+      <c r="D101" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="E101" s="25" t="s">
+      <c r="E101" s="24" t="s">
         <v>275</v>
       </c>
-      <c r="F101" s="23" t="s">
+      <c r="F101" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="G101" s="23" t="s">
+      <c r="G101" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="H101" s="23" t="s">
+      <c r="H101" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="I101" s="23" t="s">
+      <c r="I101" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="J101" s="23" t="s">
+      <c r="J101" s="22" t="s">
         <v>278</v>
       </c>
     </row>
@@ -4504,31 +4894,31 @@
       <c r="A102" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B102" s="23" t="s">
+      <c r="B102" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="C102" s="24" t="s">
+      <c r="C102" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="D102" s="25" t="s">
+      <c r="D102" s="24" t="s">
         <v>271</v>
       </c>
-      <c r="E102" s="24" t="s">
+      <c r="E102" s="23" t="s">
         <v>276</v>
       </c>
-      <c r="F102" s="23" t="s">
+      <c r="F102" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="G102" s="24" t="s">
+      <c r="G102" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="H102" s="20" t="s">
+      <c r="H102" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="I102" s="23" t="s">
+      <c r="I102" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="J102" s="23" t="s">
+      <c r="J102" s="22" t="s">
         <v>114</v>
       </c>
     </row>
@@ -4536,31 +4926,31 @@
       <c r="A103" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B103" s="23" t="s">
+      <c r="B103" s="22" t="s">
         <v>265</v>
       </c>
-      <c r="C103" s="24" t="s">
+      <c r="C103" s="23" t="s">
         <v>267</v>
       </c>
-      <c r="D103" s="25" t="s">
+      <c r="D103" s="24" t="s">
         <v>272</v>
       </c>
-      <c r="E103" s="23" t="s">
+      <c r="E103" s="22" t="s">
         <v>277</v>
       </c>
-      <c r="F103" s="23" t="s">
+      <c r="F103" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="G103" s="23" t="s">
+      <c r="G103" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="H103" s="23" t="s">
+      <c r="H103" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="I103" s="23" t="s">
+      <c r="I103" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="J103" s="23" t="s">
+      <c r="J103" s="22" t="s">
         <v>88</v>
       </c>
     </row>
@@ -4568,31 +4958,31 @@
       <c r="A104" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B104" s="18">
+      <c r="B104" s="17">
         <v>3</v>
       </c>
-      <c r="C104" s="18">
-        <v>0</v>
-      </c>
-      <c r="D104" s="18">
+      <c r="C104" s="17">
+        <v>0</v>
+      </c>
+      <c r="D104" s="17">
         <v>2</v>
       </c>
-      <c r="E104" s="18">
-        <v>1</v>
-      </c>
-      <c r="F104" s="18">
+      <c r="E104" s="17">
+        <v>1</v>
+      </c>
+      <c r="F104" s="17">
         <v>4</v>
       </c>
-      <c r="G104" s="18">
+      <c r="G104" s="17">
         <v>4</v>
       </c>
-      <c r="H104" s="18">
+      <c r="H104" s="17">
         <v>5</v>
       </c>
-      <c r="I104" s="18">
+      <c r="I104" s="17">
         <v>4</v>
       </c>
-      <c r="J104" s="18">
+      <c r="J104" s="17">
         <v>4</v>
       </c>
     </row>
@@ -4600,77 +4990,77 @@
       <c r="A105" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B105" s="18">
+      <c r="B105" s="17">
         <v>2</v>
       </c>
-      <c r="C105" s="18">
+      <c r="C105" s="17">
         <v>4</v>
       </c>
-      <c r="D105" s="18">
-        <v>1</v>
-      </c>
-      <c r="E105" s="18">
-        <v>1</v>
-      </c>
-      <c r="F105" s="18">
-        <v>1</v>
-      </c>
-      <c r="G105" s="18">
-        <v>1</v>
-      </c>
-      <c r="H105" s="18">
-        <v>0</v>
-      </c>
-      <c r="I105" s="18">
-        <v>1</v>
-      </c>
-      <c r="J105" s="18">
+      <c r="D105" s="17">
+        <v>1</v>
+      </c>
+      <c r="E105" s="17">
+        <v>1</v>
+      </c>
+      <c r="F105" s="17">
+        <v>1</v>
+      </c>
+      <c r="G105" s="17">
+        <v>1</v>
+      </c>
+      <c r="H105" s="17">
+        <v>0</v>
+      </c>
+      <c r="I105" s="17">
+        <v>1</v>
+      </c>
+      <c r="J105" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="18"/>
-      <c r="B106" s="18" t="s">
+      <c r="A106" s="17"/>
+      <c r="B106" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="C106" s="18"/>
-      <c r="D106" s="18"/>
-      <c r="E106" s="18"/>
-      <c r="F106" s="18"/>
-      <c r="G106" s="18"/>
-      <c r="H106" s="18"/>
-      <c r="I106" s="18"/>
-      <c r="J106" s="18"/>
+      <c r="C106" s="28"/>
+      <c r="D106" s="28"/>
+      <c r="E106" s="28"/>
+      <c r="F106" s="28"/>
+      <c r="G106" s="28"/>
+      <c r="H106" s="28"/>
+      <c r="I106" s="28"/>
+      <c r="J106" s="28"/>
     </row>
     <row r="107" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A107" s="18">
+      <c r="A107" s="17">
         <v>12</v>
       </c>
-      <c r="B107" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C107" s="18" t="s">
+      <c r="B107" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D107" s="18" t="s">
+      <c r="D107" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E107" s="18" t="s">
+      <c r="E107" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F107" s="18" t="s">
+      <c r="F107" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G107" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H107" s="18" t="s">
+      <c r="G107" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H107" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="I107" s="18" t="s">
+      <c r="I107" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="J107" s="19" t="s">
+      <c r="J107" s="18" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4678,31 +5068,31 @@
       <c r="A108" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B108" s="23" t="s">
+      <c r="B108" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="C108" s="25" t="s">
+      <c r="C108" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D108" s="25" t="s">
+      <c r="D108" s="24" t="s">
         <v>287</v>
       </c>
-      <c r="E108" s="23" t="s">
+      <c r="E108" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="F108" s="23" t="s">
+      <c r="F108" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="G108" s="23" t="s">
+      <c r="G108" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="H108" s="23" t="s">
+      <c r="H108" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="I108" s="23" t="s">
+      <c r="I108" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="J108" s="23" t="s">
+      <c r="J108" s="22" t="s">
         <v>286</v>
       </c>
     </row>
@@ -4710,31 +5100,31 @@
       <c r="A109" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B109" s="23" t="s">
+      <c r="B109" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="C109" s="25" t="s">
+      <c r="C109" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="D109" s="23" t="s">
+      <c r="D109" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="E109" s="23" t="s">
+      <c r="E109" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="F109" s="23" t="s">
+      <c r="F109" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="G109" s="23" t="s">
+      <c r="G109" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="H109" s="23" t="s">
+      <c r="H109" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="I109" s="23" t="s">
+      <c r="I109" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="J109" s="23" t="s">
+      <c r="J109" s="22" t="s">
         <v>300</v>
       </c>
     </row>
@@ -4742,31 +5132,31 @@
       <c r="A110" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B110" s="23" t="s">
+      <c r="B110" s="22" t="s">
         <v>284</v>
       </c>
-      <c r="C110" s="23" t="s">
+      <c r="C110" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="D110" s="26" t="s">
+      <c r="D110" s="25" t="s">
         <v>289</v>
       </c>
-      <c r="E110" s="24" t="s">
+      <c r="E110" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="F110" s="21" t="s">
+      <c r="F110" s="20" t="s">
         <v>297</v>
       </c>
-      <c r="G110" s="23" t="s">
+      <c r="G110" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H110" s="23" t="s">
+      <c r="H110" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="I110" s="23" t="s">
+      <c r="I110" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J110" s="23" t="s">
+      <c r="J110" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4774,31 +5164,31 @@
       <c r="A111" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B111" s="23" t="s">
+      <c r="B111" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="C111" s="25" t="s">
+      <c r="C111" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="D111" s="22" t="s">
+      <c r="D111" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="E111" s="23" t="s">
+      <c r="E111" s="22" t="s">
         <v>293</v>
       </c>
-      <c r="F111" s="24" t="s">
+      <c r="F111" s="23" t="s">
         <v>298</v>
       </c>
-      <c r="G111" s="23" t="s">
+      <c r="G111" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="H111" s="23" t="s">
+      <c r="H111" s="22" t="s">
         <v>304</v>
       </c>
-      <c r="I111" s="23" t="s">
+      <c r="I111" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="J111" s="23" t="s">
+      <c r="J111" s="22" t="s">
         <v>303</v>
       </c>
     </row>
@@ -4806,31 +5196,31 @@
       <c r="A112" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B112" s="23" t="s">
+      <c r="B112" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="C112" s="25" t="s">
+      <c r="C112" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="D112" s="25" t="s">
+      <c r="D112" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="E112" s="25" t="s">
+      <c r="E112" s="24" t="s">
         <v>294</v>
       </c>
-      <c r="F112" s="24" t="s">
+      <c r="F112" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="G112" s="23" t="s">
+      <c r="G112" s="22" t="s">
         <v>302</v>
       </c>
-      <c r="H112" s="23" t="s">
+      <c r="H112" s="22" t="s">
         <v>305</v>
       </c>
-      <c r="I112" s="24" t="s">
+      <c r="I112" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="J112" s="24" t="s">
+      <c r="J112" s="23" t="s">
         <v>306</v>
       </c>
     </row>
@@ -4838,31 +5228,31 @@
       <c r="A113" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B113" s="18">
+      <c r="B113" s="17">
         <v>5</v>
       </c>
-      <c r="C113" s="18">
-        <v>1</v>
-      </c>
-      <c r="D113" s="18">
-        <v>1</v>
-      </c>
-      <c r="E113" s="18">
+      <c r="C113" s="17">
+        <v>1</v>
+      </c>
+      <c r="D113" s="17">
+        <v>1</v>
+      </c>
+      <c r="E113" s="17">
         <v>3</v>
       </c>
-      <c r="F113" s="18">
+      <c r="F113" s="17">
         <v>2</v>
       </c>
-      <c r="G113" s="18">
+      <c r="G113" s="17">
         <v>5</v>
       </c>
-      <c r="H113" s="18">
+      <c r="H113" s="17">
         <v>5</v>
       </c>
-      <c r="I113" s="18">
+      <c r="I113" s="17">
         <v>4</v>
       </c>
-      <c r="J113" s="18">
+      <c r="J113" s="17">
         <v>4</v>
       </c>
     </row>
@@ -4873,73 +5263,73 @@
       <c r="B114" s="1">
         <v>0</v>
       </c>
-      <c r="C114" s="18">
-        <v>0</v>
-      </c>
-      <c r="D114" s="18">
-        <v>0</v>
-      </c>
-      <c r="E114" s="18">
-        <v>1</v>
-      </c>
-      <c r="F114" s="18">
+      <c r="C114" s="17">
+        <v>0</v>
+      </c>
+      <c r="D114" s="17">
+        <v>0</v>
+      </c>
+      <c r="E114" s="17">
+        <v>1</v>
+      </c>
+      <c r="F114" s="17">
         <v>3</v>
       </c>
-      <c r="G114" s="18">
-        <v>0</v>
-      </c>
-      <c r="H114" s="18">
-        <v>0</v>
-      </c>
-      <c r="I114" s="18">
-        <v>1</v>
-      </c>
-      <c r="J114" s="18">
+      <c r="G114" s="17">
+        <v>0</v>
+      </c>
+      <c r="H114" s="17">
+        <v>0</v>
+      </c>
+      <c r="I114" s="17">
+        <v>1</v>
+      </c>
+      <c r="J114" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B115" s="16" t="s">
+      <c r="B115" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="C115" s="16"/>
-      <c r="D115" s="16"/>
-      <c r="E115" s="16"/>
-      <c r="F115" s="16"/>
-      <c r="G115" s="16"/>
-      <c r="H115" s="16"/>
-      <c r="I115" s="16"/>
-      <c r="J115" s="16"/>
+      <c r="C115" s="28"/>
+      <c r="D115" s="28"/>
+      <c r="E115" s="28"/>
+      <c r="F115" s="28"/>
+      <c r="G115" s="28"/>
+      <c r="H115" s="28"/>
+      <c r="I115" s="28"/>
+      <c r="J115" s="28"/>
     </row>
     <row r="116" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>13</v>
       </c>
-      <c r="B116" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C116" s="18" t="s">
+      <c r="B116" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C116" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D116" s="18" t="s">
+      <c r="D116" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E116" s="18" t="s">
+      <c r="E116" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F116" s="18" t="s">
+      <c r="F116" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G116" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H116" s="18" t="s">
+      <c r="G116" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H116" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="I116" s="18" t="s">
+      <c r="I116" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="J116" s="19" t="s">
+      <c r="J116" s="18" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4947,31 +5337,31 @@
       <c r="A117" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B117" s="25" t="s">
+      <c r="B117" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C117" s="25" t="s">
+      <c r="C117" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="D117" s="18" t="s">
+      <c r="D117" s="28" t="s">
         <v>323</v>
       </c>
-      <c r="E117" s="25" t="s">
+      <c r="E117" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="F117" s="24" t="s">
+      <c r="F117" s="23" t="s">
         <v>295</v>
       </c>
-      <c r="G117" s="23" t="s">
+      <c r="G117" s="22" t="s">
         <v>319</v>
       </c>
-      <c r="H117" s="16" t="s">
+      <c r="H117" s="28" t="s">
         <v>322</v>
       </c>
-      <c r="I117" s="16" t="s">
+      <c r="I117" s="28" t="s">
         <v>322</v>
       </c>
-      <c r="J117" s="16" t="s">
+      <c r="J117" s="28" t="s">
         <v>322</v>
       </c>
     </row>
@@ -4979,97 +5369,97 @@
       <c r="A118" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B118" s="25" t="s">
+      <c r="B118" s="24" t="s">
         <v>308</v>
       </c>
-      <c r="C118" s="25" t="s">
+      <c r="C118" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D118" s="18"/>
-      <c r="E118" s="25" t="s">
+      <c r="D118" s="28"/>
+      <c r="E118" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="F118" s="24" t="s">
+      <c r="F118" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="G118" s="23" t="s">
+      <c r="G118" s="22" t="s">
         <v>320</v>
       </c>
-      <c r="H118" s="16"/>
-      <c r="I118" s="16"/>
-      <c r="J118" s="16"/>
+      <c r="H118" s="28"/>
+      <c r="I118" s="28"/>
+      <c r="J118" s="28"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B119" s="25" t="s">
+      <c r="B119" s="24" t="s">
         <v>309</v>
       </c>
-      <c r="C119" s="25" t="s">
+      <c r="C119" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D119" s="18"/>
-      <c r="E119" s="22" t="s">
+      <c r="D119" s="28"/>
+      <c r="E119" s="21" t="s">
         <v>316</v>
       </c>
-      <c r="F119" s="23" t="s">
+      <c r="F119" s="22" t="s">
         <v>297</v>
       </c>
-      <c r="G119" s="24" t="s">
+      <c r="G119" s="23" t="s">
         <v>295</v>
       </c>
-      <c r="H119" s="16"/>
-      <c r="I119" s="16"/>
-      <c r="J119" s="16"/>
+      <c r="H119" s="28"/>
+      <c r="I119" s="28"/>
+      <c r="J119" s="28"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B120" s="25" t="s">
+      <c r="B120" s="24" t="s">
         <v>310</v>
       </c>
-      <c r="C120" s="25" t="s">
+      <c r="C120" s="24" t="s">
         <v>313</v>
       </c>
-      <c r="D120" s="18"/>
-      <c r="E120" s="23" t="s">
+      <c r="D120" s="28"/>
+      <c r="E120" s="22" t="s">
         <v>317</v>
       </c>
-      <c r="F120" s="23" t="s">
+      <c r="F120" s="22" t="s">
         <v>298</v>
       </c>
-      <c r="G120" s="24" t="s">
+      <c r="G120" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="H120" s="16"/>
-      <c r="I120" s="16"/>
-      <c r="J120" s="16"/>
+      <c r="H120" s="28"/>
+      <c r="I120" s="28"/>
+      <c r="J120" s="28"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B121" s="25" t="s">
+      <c r="B121" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="C121" s="25" t="s">
+      <c r="C121" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="D121" s="18"/>
-      <c r="E121" s="25" t="s">
+      <c r="D121" s="28"/>
+      <c r="E121" s="24" t="s">
         <v>318</v>
       </c>
-      <c r="F121" s="24" t="s">
+      <c r="F121" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="G121" s="23" t="s">
+      <c r="G121" s="22" t="s">
         <v>321</v>
       </c>
-      <c r="H121" s="16"/>
-      <c r="I121" s="16"/>
-      <c r="J121" s="16"/>
+      <c r="H121" s="28"/>
+      <c r="I121" s="28"/>
+      <c r="J121" s="28"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
@@ -5112,47 +5502,47 @@
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B124" s="16" t="s">
+      <c r="B124" s="28" t="s">
         <v>328</v>
       </c>
-      <c r="C124" s="16"/>
-      <c r="D124" s="16"/>
-      <c r="E124" s="16"/>
-      <c r="F124" s="16"/>
-      <c r="G124" s="16"/>
-      <c r="H124" s="16"/>
-      <c r="I124" s="16"/>
-      <c r="J124" s="16"/>
+      <c r="C124" s="28"/>
+      <c r="D124" s="28"/>
+      <c r="E124" s="28"/>
+      <c r="F124" s="28"/>
+      <c r="G124" s="28"/>
+      <c r="H124" s="28"/>
+      <c r="I124" s="28"/>
+      <c r="J124" s="28"/>
     </row>
     <row r="125" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>14</v>
       </c>
-      <c r="B125" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C125" s="18" t="s">
+      <c r="B125" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C125" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D125" s="18" t="s">
+      <c r="D125" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E125" s="18" t="s">
+      <c r="E125" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F125" s="18" t="s">
+      <c r="F125" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G125" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H125" s="18" t="s">
+      <c r="G125" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H125" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="I125" s="18" t="s">
+      <c r="I125" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="J125" s="19" t="s">
+      <c r="J125" s="18" t="s">
         <v>37</v>
       </c>
     </row>
@@ -5317,6 +5707,9 @@
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>324</v>
+      </c>
       <c r="B131" s="1">
         <v>5</v>
       </c>
@@ -5332,8 +5725,17 @@
       <c r="H131" s="1">
         <v>3</v>
       </c>
+      <c r="I131" s="1">
+        <v>4</v>
+      </c>
+      <c r="J131" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>326</v>
+      </c>
       <c r="B132" s="1">
         <v>0</v>
       </c>
@@ -5349,49 +5751,55 @@
       <c r="H132" s="1">
         <v>1</v>
       </c>
+      <c r="I132" s="1">
+        <v>1</v>
+      </c>
+      <c r="J132" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B133" s="16" t="s">
+      <c r="B133" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="C133" s="16"/>
-      <c r="D133" s="16"/>
-      <c r="E133" s="16"/>
-      <c r="F133" s="16"/>
-      <c r="G133" s="16"/>
-      <c r="H133" s="16"/>
-      <c r="I133" s="16"/>
-      <c r="J133" s="16"/>
+      <c r="C133" s="28"/>
+      <c r="D133" s="28"/>
+      <c r="E133" s="28"/>
+      <c r="F133" s="28"/>
+      <c r="G133" s="28"/>
+      <c r="H133" s="28"/>
+      <c r="I133" s="28"/>
+      <c r="J133" s="28"/>
     </row>
     <row r="134" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>15</v>
       </c>
-      <c r="B134" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C134" s="18" t="s">
+      <c r="B134" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C134" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D134" s="18" t="s">
+      <c r="D134" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E134" s="18" t="s">
+      <c r="E134" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F134" s="18" t="s">
+      <c r="F134" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G134" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H134" s="18" t="s">
+      <c r="G134" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H134" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="I134" s="18" t="s">
+      <c r="I134" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="J134" s="19" t="s">
+      <c r="J134" s="18" t="s">
         <v>37</v>
       </c>
     </row>
@@ -5414,7 +5822,7 @@
       <c r="F135" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="G135" s="27" t="s">
+      <c r="G135" s="26" t="s">
         <v>368</v>
       </c>
       <c r="H135" s="6" t="s">
@@ -5556,6 +5964,9 @@
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>324</v>
+      </c>
       <c r="B140" s="1">
         <v>5</v>
       </c>
@@ -5585,6 +5996,9 @@
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>326</v>
+      </c>
       <c r="B141" s="1">
         <v>0</v>
       </c>
@@ -5613,8 +6027,1253 @@
         <v>0</v>
       </c>
     </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143" s="2"/>
+      <c r="B143" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="C143" s="28"/>
+      <c r="D143" s="28"/>
+      <c r="E143" s="28"/>
+      <c r="F143" s="28"/>
+      <c r="G143" s="28"/>
+      <c r="H143" s="28"/>
+      <c r="I143" s="28"/>
+      <c r="J143" s="28"/>
+    </row>
+    <row r="144" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="2">
+        <v>16</v>
+      </c>
+      <c r="B144" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C144" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D144" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E144" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F144" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G144" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H144" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="I144" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J144" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="E145" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="F145" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G145" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="H145" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="I145" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J145" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="E146" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="F146" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G146" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H146" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="I146" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="J146" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="C147" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D147" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="E147" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="F147" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G147" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="H147" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="I147" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="J147" s="6" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D148" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="E148" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="F148" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G148" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="H148" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I148" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="J148" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="E149" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="F149" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G149" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H149" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="I149" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="J149" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B150" s="1">
+        <v>3</v>
+      </c>
+      <c r="C150" s="1">
+        <v>1</v>
+      </c>
+      <c r="D150" s="1">
+        <v>0</v>
+      </c>
+      <c r="E150" s="1">
+        <v>3</v>
+      </c>
+      <c r="F150" s="1">
+        <v>3</v>
+      </c>
+      <c r="G150" s="1">
+        <v>5</v>
+      </c>
+      <c r="H150" s="1">
+        <v>4</v>
+      </c>
+      <c r="I150" s="1">
+        <v>4</v>
+      </c>
+      <c r="J150" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B151" s="1">
+        <v>2</v>
+      </c>
+      <c r="C151" s="1">
+        <v>0</v>
+      </c>
+      <c r="D151" s="1">
+        <v>1</v>
+      </c>
+      <c r="E151" s="1">
+        <v>1</v>
+      </c>
+      <c r="F151" s="1">
+        <v>2</v>
+      </c>
+      <c r="G151" s="1">
+        <v>0</v>
+      </c>
+      <c r="H151" s="1">
+        <v>1</v>
+      </c>
+      <c r="I151" s="1">
+        <v>1</v>
+      </c>
+      <c r="J151" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A153" s="2"/>
+      <c r="B153" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C153" s="28"/>
+      <c r="D153" s="28"/>
+      <c r="E153" s="28"/>
+      <c r="F153" s="28"/>
+      <c r="G153" s="28"/>
+      <c r="H153" s="28"/>
+      <c r="I153" s="28"/>
+      <c r="J153" s="28"/>
+    </row>
+    <row r="154" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>17</v>
+      </c>
+      <c r="B154" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C154" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D154" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E154" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F154" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G154" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H154" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="I154" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J154" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D155" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="E155" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="F155" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="G155" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H155" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="I155" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="J155" s="6" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B156" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="C156" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D156" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="E156" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="F156" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G156" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="H156" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="I156" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="J156" s="6" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B157" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E157" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="F157" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G157" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="H157" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="I157" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="J157" s="5" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B158" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="E158" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="F158" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G158" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="H158" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="I158" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="J158" s="6" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B159" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C159" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D159" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="E159" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="F159" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="G159" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H159" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="I159" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="J159" s="6" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B160" s="1">
+        <v>2</v>
+      </c>
+      <c r="C160" s="1">
+        <v>0</v>
+      </c>
+      <c r="D160" s="1">
+        <v>0</v>
+      </c>
+      <c r="E160" s="1">
+        <v>0</v>
+      </c>
+      <c r="F160" s="1">
+        <v>1</v>
+      </c>
+      <c r="G160" s="1">
+        <v>2</v>
+      </c>
+      <c r="H160" s="1">
+        <v>2</v>
+      </c>
+      <c r="I160" s="1">
+        <v>4</v>
+      </c>
+      <c r="J160" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B161" s="1">
+        <v>2</v>
+      </c>
+      <c r="C161" s="1">
+        <v>0</v>
+      </c>
+      <c r="D161" s="1">
+        <v>0</v>
+      </c>
+      <c r="E161" s="1">
+        <v>2</v>
+      </c>
+      <c r="F161" s="1">
+        <v>1</v>
+      </c>
+      <c r="G161" s="1">
+        <v>3</v>
+      </c>
+      <c r="H161" s="1">
+        <v>2</v>
+      </c>
+      <c r="I161" s="1">
+        <v>1</v>
+      </c>
+      <c r="J161" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163" s="2"/>
+      <c r="B163" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="C163" s="28"/>
+      <c r="D163" s="28"/>
+      <c r="E163" s="28"/>
+      <c r="F163" s="28"/>
+      <c r="G163" s="28"/>
+      <c r="H163" s="28"/>
+      <c r="I163" s="28"/>
+      <c r="J163" s="28"/>
+    </row>
+    <row r="164" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="2">
+        <v>18</v>
+      </c>
+      <c r="B164" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C164" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D164" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E164" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F164" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G164" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H164" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="I164" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J164" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B165" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="C165" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D165" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="E165" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="F165" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G165" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H165" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="I165" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J165" s="6" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B166" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="C166" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D166" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="E166" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="F166" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="G166" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="H166" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="I166" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="J166" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B167" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="C167" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="E167" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="F167" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G167" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H167" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="I167" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J167" s="6" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B168" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="C168" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="E168" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="F168" s="26" t="s">
+        <v>433</v>
+      </c>
+      <c r="G168" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="H168" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="I168" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="J168" s="5" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D169" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="E169" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="F169" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="G169" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="H169" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="I169" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="J169" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B170" s="1">
+        <v>4</v>
+      </c>
+      <c r="C170" s="1">
+        <v>0</v>
+      </c>
+      <c r="D170" s="1">
+        <v>1</v>
+      </c>
+      <c r="E170" s="1">
+        <v>0</v>
+      </c>
+      <c r="F170" s="1">
+        <v>1</v>
+      </c>
+      <c r="G170" s="1">
+        <v>1</v>
+      </c>
+      <c r="H170" s="1">
+        <v>3</v>
+      </c>
+      <c r="I170" s="1">
+        <v>2</v>
+      </c>
+      <c r="J170" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B171" s="1">
+        <v>0</v>
+      </c>
+      <c r="C171" s="1">
+        <v>0</v>
+      </c>
+      <c r="D171" s="1">
+        <v>1</v>
+      </c>
+      <c r="E171" s="1">
+        <v>0</v>
+      </c>
+      <c r="F171" s="1">
+        <v>4</v>
+      </c>
+      <c r="G171" s="1">
+        <v>4</v>
+      </c>
+      <c r="H171" s="1">
+        <v>2</v>
+      </c>
+      <c r="I171" s="1">
+        <v>3</v>
+      </c>
+      <c r="J171" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A174" s="2"/>
+      <c r="B174" s="28" t="s">
+        <v>442</v>
+      </c>
+      <c r="C174" s="28"/>
+      <c r="D174" s="28"/>
+      <c r="E174" s="28"/>
+      <c r="F174" s="28"/>
+      <c r="G174" s="28"/>
+      <c r="H174" s="28"/>
+      <c r="I174" s="28"/>
+      <c r="J174" s="28"/>
+    </row>
+    <row r="175" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="2">
+        <v>19</v>
+      </c>
+      <c r="B175" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C175" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D175" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E175" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F175" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G175" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H175" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="I175" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J175" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B176" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="C176" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D176" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="E176" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="F176" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G176" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H176" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="I176" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="J176" s="28" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D177" s="28"/>
+      <c r="E177" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="F177" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G177" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="H177" s="28"/>
+      <c r="I177" s="28"/>
+      <c r="J177" s="28"/>
+    </row>
+    <row r="178" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="C178" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="D178" s="28"/>
+      <c r="E178" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="F178" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G178" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="H178" s="28"/>
+      <c r="I178" s="28"/>
+      <c r="J178" s="28"/>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="C179" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D179" s="28"/>
+      <c r="E179" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="F179" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G179" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="H179" s="28"/>
+      <c r="I179" s="28"/>
+      <c r="J179" s="28"/>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D180" s="28"/>
+      <c r="E180" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="F180" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="G180" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="H180" s="28"/>
+      <c r="I180" s="28"/>
+      <c r="J180" s="28"/>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B181" s="1">
+        <v>2</v>
+      </c>
+      <c r="C181" s="1">
+        <v>0</v>
+      </c>
+      <c r="E181" s="1">
+        <v>1</v>
+      </c>
+      <c r="F181" s="1">
+        <v>1</v>
+      </c>
+      <c r="G181" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B182" s="1">
+        <v>3</v>
+      </c>
+      <c r="C182" s="1">
+        <v>0</v>
+      </c>
+      <c r="E182" s="1">
+        <v>3</v>
+      </c>
+      <c r="F182" s="1">
+        <v>0</v>
+      </c>
+      <c r="G182" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A183" s="2"/>
+      <c r="B183" s="28" t="s">
+        <v>457</v>
+      </c>
+      <c r="C183" s="28"/>
+      <c r="D183" s="28"/>
+      <c r="E183" s="28"/>
+      <c r="F183" s="28"/>
+      <c r="G183" s="28"/>
+      <c r="H183" s="28"/>
+      <c r="I183" s="28"/>
+      <c r="J183" s="28"/>
+    </row>
+    <row r="184" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A184" s="2">
+        <v>20</v>
+      </c>
+      <c r="B184" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C184" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D184" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E184" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F184" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G184" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H184" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="I184" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J184" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B185" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="C185" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="D185" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="E185" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="F185" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G185" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H185" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="I185" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="J185" s="28" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B186" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="C186" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D186" s="28"/>
+      <c r="E186" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="F186" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G186" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="H186" s="28"/>
+      <c r="I186" s="28"/>
+      <c r="J186" s="28"/>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B187" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="C187" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="D187" s="28"/>
+      <c r="E187" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="F187" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G187" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="H187" s="28"/>
+      <c r="I187" s="28"/>
+      <c r="J187" s="28"/>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="C188" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D188" s="28"/>
+      <c r="E188" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="F188" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G188" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="H188" s="28"/>
+      <c r="I188" s="28"/>
+      <c r="J188" s="28"/>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B189" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="C189" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="D189" s="28"/>
+      <c r="E189" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F189" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="G189" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="H189" s="28"/>
+      <c r="I189" s="28"/>
+      <c r="J189" s="28"/>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B190" s="1">
+        <v>4</v>
+      </c>
+      <c r="C190" s="1">
+        <v>2</v>
+      </c>
+      <c r="E190" s="1">
+        <v>3</v>
+      </c>
+      <c r="F190" s="1">
+        <v>0</v>
+      </c>
+      <c r="G190" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B191" s="1">
+        <v>1</v>
+      </c>
+      <c r="C191" s="1">
+        <v>3</v>
+      </c>
+      <c r="E191" s="1">
+        <v>2</v>
+      </c>
+      <c r="F191" s="1">
+        <v>1</v>
+      </c>
+      <c r="G191" s="1">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="39">
+    <mergeCell ref="H185:H189"/>
+    <mergeCell ref="I185:I189"/>
+    <mergeCell ref="J185:J189"/>
+    <mergeCell ref="D185:D189"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B153:J153"/>
+    <mergeCell ref="B163:J163"/>
+    <mergeCell ref="B174:J174"/>
+    <mergeCell ref="B183:J183"/>
+    <mergeCell ref="D176:D180"/>
+    <mergeCell ref="H176:H180"/>
+    <mergeCell ref="I176:I180"/>
+    <mergeCell ref="J176:J180"/>
+    <mergeCell ref="B52:J52"/>
+    <mergeCell ref="B43:J43"/>
+    <mergeCell ref="B34:J34"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="B143:J143"/>
+    <mergeCell ref="D117:D121"/>
+    <mergeCell ref="B106:J106"/>
+    <mergeCell ref="B97:J97"/>
+    <mergeCell ref="B88:J88"/>
     <mergeCell ref="B124:J124"/>
     <mergeCell ref="B133:J133"/>
     <mergeCell ref="B1:J1"/>
@@ -5624,6 +7283,13 @@
     <mergeCell ref="H117:H121"/>
     <mergeCell ref="I117:I121"/>
     <mergeCell ref="J117:J121"/>
+    <mergeCell ref="D63:D67"/>
+    <mergeCell ref="H63:H67"/>
+    <mergeCell ref="I63:I67"/>
+    <mergeCell ref="J63:J67"/>
+    <mergeCell ref="B79:J79"/>
+    <mergeCell ref="B70:J70"/>
+    <mergeCell ref="B61:J61"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B6:J6">

</xml_diff>